<commit_message>
Second commit of Eletter
</commit_message>
<xml_diff>
--- a/bin/Externaldata/TestData.xlsx
+++ b/bin/Externaldata/TestData.xlsx
@@ -4,12 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="10755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="10755" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ExitLetter" sheetId="1" r:id="rId1"/>
     <sheet name="Internshipletter" sheetId="2" r:id="rId2"/>
-    <sheet name="Offerletter" sheetId="3" r:id="rId3"/>
+    <sheet name="SalaryRevisionLetter" sheetId="8" r:id="rId3"/>
+    <sheet name="ProjectPolicyLetter" sheetId="9" r:id="rId4"/>
+    <sheet name="Offerletter" sheetId="3" r:id="rId5"/>
+    <sheet name="HRPolicyLetter" sheetId="4" r:id="rId6"/>
+    <sheet name="ITPolicyLetter" sheetId="10" r:id="rId7"/>
+    <sheet name="DeliveryPolicyLetter" sheetId="11" r:id="rId8"/>
+    <sheet name="BDPolicyLetter" sheetId="5" r:id="rId9"/>
+    <sheet name="ConsultantOfferLetter" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:W33"/>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="60">
   <si>
     <t>Salutation</t>
   </si>
@@ -153,9 +160,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>P.Vijay Kumar</t>
-  </si>
-  <si>
     <t>Offer validity</t>
   </si>
   <si>
@@ -166,6 +170,45 @@
   </si>
   <si>
     <t>18-02-2021</t>
+  </si>
+  <si>
+    <t>P. Vijay Kumar</t>
+  </si>
+  <si>
+    <t>Employee Id</t>
+  </si>
+  <si>
+    <t>Edit name</t>
+  </si>
+  <si>
+    <t>Notice period Month</t>
+  </si>
+  <si>
+    <t>Reporting date</t>
+  </si>
+  <si>
+    <t>21-02-2020</t>
+  </si>
+  <si>
+    <t>Edit location</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Increment in Effect date</t>
+  </si>
+  <si>
+    <t>10-02-2020</t>
+  </si>
+  <si>
+    <t>Salary Incremented from</t>
+  </si>
+  <si>
+    <t>Salary Incremented to</t>
   </si>
 </sst>
 </file>
@@ -211,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -234,12 +277,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -250,6 +304,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +611,7 @@
     <col min="13" max="13" width="35.42578125" customWidth="1"/>
     <col min="14" max="14" width="24.28515625" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -603,6 +663,9 @@
       <c r="P1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="2" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -650,6 +713,9 @@
       </c>
       <c r="P2" t="s">
         <v>37</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -682,6 +748,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
+    <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1"/>
@@ -692,12 +759,146 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,10 +1020,267 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="48.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2">
+        <v>30000</v>
+      </c>
+      <c r="E2">
+        <v>40000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +1295,7 @@
     <col min="11" max="11" width="35.42578125" customWidth="1"/>
     <col min="12" max="12" width="24.28515625" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -862,10 +1321,10 @@
         <v>10</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>19</v>
@@ -881,6 +1340,9 @@
       </c>
       <c r="N1" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
@@ -891,7 +1353,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D2" s="4">
         <v>21</v>
@@ -906,10 +1368,10 @@
         <v>30000</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
@@ -925,6 +1387,9 @@
       </c>
       <c r="N2" t="s">
         <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
@@ -960,4 +1425,544 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="6" width="16" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4">
+        <v>21</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Eletter testing first commit
</commit_message>
<xml_diff>
--- a/bin/Externaldata/TestData.xlsx
+++ b/bin/Externaldata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="10755" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="10755" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ExitLetter" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="ConsultantOfferLetter" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:W33"/>
+  <oleSize ref="A1:J33"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="62">
   <si>
     <t>Salutation</t>
   </si>
@@ -115,12 +115,6 @@
     <t>Internship end date date</t>
   </si>
   <si>
-    <t>25-05-2020</t>
-  </si>
-  <si>
-    <t>TYC1012000</t>
-  </si>
-  <si>
     <t>Fresher</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>18-02-2021</t>
   </si>
   <si>
-    <t>P. Vijay Kumar</t>
-  </si>
-  <si>
     <t>Employee Id</t>
   </si>
   <si>
@@ -190,25 +181,40 @@
     <t>21-02-2020</t>
   </si>
   <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>Increment in Effect date</t>
+  </si>
+  <si>
+    <t>10-02-2020</t>
+  </si>
+  <si>
+    <t>Salary Incremented from</t>
+  </si>
+  <si>
+    <t>Salary Incremented to</t>
+  </si>
+  <si>
     <t>Edit location</t>
   </si>
   <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>File Path</t>
-  </si>
-  <si>
-    <t>Increment in Effect date</t>
-  </si>
-  <si>
-    <t>10-02-2020</t>
-  </si>
-  <si>
-    <t>Salary Incremented from</t>
-  </si>
-  <si>
-    <t>Salary Incremented to</t>
+    <t>TYC101200</t>
+  </si>
+  <si>
+    <t>P Vijay Kumar</t>
+  </si>
+  <si>
+    <t>TYC102000</t>
+  </si>
+  <si>
+    <t>18-02-2022</t>
+  </si>
+  <si>
+    <t>25-08-2022</t>
+  </si>
+  <si>
+    <t>P  Vijay Kumar</t>
   </si>
 </sst>
 </file>
@@ -593,7 +599,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,19 +658,19 @@
         <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -703,19 +709,19 @@
         <v>20</v>
       </c>
       <c r="M2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" t="s">
         <v>38</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:19" customFormat="1" x14ac:dyDescent="0.25">
@@ -763,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,31 +802,31 @@
         <v>7</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -840,28 +846,28 @@
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
         <v>38</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -898,7 +904,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,19 +949,19 @@
         <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -966,37 +972,37 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
         <v>38</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1022,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,34 +1051,34 @@
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1080,10 +1086,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <v>30000</v>
@@ -1095,19 +1101,19 @@
         <v>20</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
         <v>38</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1142,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -1177,25 +1183,25 @@
         <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1206,34 +1212,34 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1279,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,10 +1312,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -1321,28 +1327,28 @@
         <v>10</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
@@ -1353,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D2" s="4">
         <v>21</v>
@@ -1368,28 +1374,28 @@
         <v>30000</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
         <v>38</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:21" customFormat="1" x14ac:dyDescent="0.25">
@@ -1432,7 +1438,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1462,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -1465,25 +1471,25 @@
         <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1494,7 +1500,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
@@ -1503,25 +1509,25 @@
         <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1556,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -1591,25 +1597,25 @@
         <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1620,7 +1626,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
@@ -1629,25 +1635,25 @@
         <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1691,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,9 +1715,10 @@
     <col min="9" max="9" width="24.28515625" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="54.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1719,7 +1726,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -1728,28 +1735,34 @@
         <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1757,7 +1770,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
@@ -1766,28 +1779,34 @@
         <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1796,7 +1815,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1805,18 +1824,18 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
@@ -1830,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,10 +1876,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -1869,28 +1888,28 @@
         <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="I1" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1901,10 +1920,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>13</v>
@@ -1916,25 +1935,25 @@
         <v>21</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s">
         <v>38</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>